<commit_message>
Temp for 201 & 202  With Crt
</commit_message>
<xml_diff>
--- a/vishnu pavi/27.04.2025/Trn201Movt (1).xlsx
+++ b/vishnu pavi/27.04.2025/Trn201Movt (1).xlsx
@@ -1730,3130 +1730,3916 @@
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="10"/>
       <c r="E221" s="10"/>
+      <c r="H221" s="10"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="10"/>
       <c r="E222" s="10"/>
+      <c r="H222" s="10"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="10"/>
       <c r="E223" s="10"/>
+      <c r="H223" s="10"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="10"/>
       <c r="E224" s="10"/>
+      <c r="H224" s="10"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="10"/>
       <c r="E225" s="10"/>
+      <c r="H225" s="10"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="10"/>
       <c r="E226" s="10"/>
+      <c r="H226" s="10"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="10"/>
       <c r="E227" s="10"/>
+      <c r="H227" s="10"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="10"/>
       <c r="E228" s="10"/>
+      <c r="H228" s="10"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="10"/>
       <c r="E229" s="10"/>
+      <c r="H229" s="10"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="10"/>
       <c r="E230" s="10"/>
+      <c r="H230" s="10"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="10"/>
       <c r="E231" s="10"/>
+      <c r="H231" s="10"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
       <c r="A232" s="10"/>
       <c r="E232" s="10"/>
+      <c r="H232" s="10"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="10"/>
       <c r="E233" s="10"/>
+      <c r="H233" s="10"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="10"/>
       <c r="E234" s="10"/>
+      <c r="H234" s="10"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="10"/>
       <c r="E235" s="10"/>
+      <c r="H235" s="10"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
       <c r="A236" s="10"/>
       <c r="E236" s="10"/>
+      <c r="H236" s="10"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
       <c r="A237" s="10"/>
       <c r="E237" s="10"/>
+      <c r="H237" s="10"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="10"/>
       <c r="E238" s="10"/>
+      <c r="H238" s="10"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="10"/>
       <c r="E239" s="10"/>
+      <c r="H239" s="10"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="10"/>
       <c r="E240" s="10"/>
+      <c r="H240" s="10"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
       <c r="A241" s="10"/>
       <c r="E241" s="10"/>
+      <c r="H241" s="10"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="10"/>
       <c r="E242" s="10"/>
+      <c r="H242" s="10"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="10"/>
       <c r="E243" s="10"/>
+      <c r="H243" s="10"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="10"/>
       <c r="E244" s="10"/>
+      <c r="H244" s="10"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="10"/>
       <c r="E245" s="10"/>
+      <c r="H245" s="10"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
       <c r="A246" s="10"/>
       <c r="E246" s="10"/>
+      <c r="H246" s="10"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
       <c r="A247" s="10"/>
       <c r="E247" s="10"/>
+      <c r="H247" s="10"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
       <c r="A248" s="10"/>
       <c r="E248" s="10"/>
+      <c r="H248" s="10"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
       <c r="A249" s="10"/>
       <c r="E249" s="10"/>
+      <c r="H249" s="10"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
       <c r="A250" s="10"/>
       <c r="E250" s="10"/>
+      <c r="H250" s="10"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
       <c r="A251" s="10"/>
       <c r="E251" s="10"/>
+      <c r="H251" s="10"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
       <c r="A252" s="10"/>
       <c r="E252" s="10"/>
+      <c r="H252" s="10"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
       <c r="A253" s="10"/>
       <c r="E253" s="10"/>
+      <c r="H253" s="10"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
       <c r="A254" s="10"/>
       <c r="E254" s="10"/>
+      <c r="H254" s="10"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
       <c r="A255" s="10"/>
       <c r="E255" s="10"/>
+      <c r="H255" s="10"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
       <c r="A256" s="10"/>
       <c r="E256" s="10"/>
+      <c r="H256" s="10"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
       <c r="A257" s="10"/>
       <c r="E257" s="10"/>
+      <c r="H257" s="10"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
       <c r="A258" s="10"/>
       <c r="E258" s="10"/>
+      <c r="H258" s="10"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
       <c r="A259" s="10"/>
       <c r="E259" s="10"/>
+      <c r="H259" s="10"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
       <c r="A260" s="10"/>
       <c r="E260" s="10"/>
+      <c r="H260" s="10"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
       <c r="A261" s="10"/>
       <c r="E261" s="10"/>
+      <c r="H261" s="10"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
       <c r="A262" s="10"/>
       <c r="E262" s="10"/>
+      <c r="H262" s="10"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
       <c r="A263" s="10"/>
       <c r="E263" s="10"/>
+      <c r="H263" s="10"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
       <c r="A264" s="10"/>
       <c r="E264" s="10"/>
+      <c r="H264" s="10"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
       <c r="A265" s="10"/>
       <c r="E265" s="10"/>
+      <c r="H265" s="10"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
       <c r="A266" s="10"/>
       <c r="E266" s="10"/>
+      <c r="H266" s="10"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
       <c r="A267" s="10"/>
       <c r="E267" s="10"/>
+      <c r="H267" s="10"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
       <c r="A268" s="10"/>
       <c r="E268" s="10"/>
+      <c r="H268" s="10"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
       <c r="A269" s="10"/>
       <c r="E269" s="10"/>
+      <c r="H269" s="10"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
       <c r="A270" s="10"/>
       <c r="E270" s="10"/>
+      <c r="H270" s="10"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
       <c r="A271" s="10"/>
       <c r="E271" s="10"/>
+      <c r="H271" s="10"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
       <c r="A272" s="10"/>
       <c r="E272" s="10"/>
+      <c r="H272" s="10"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
       <c r="A273" s="10"/>
       <c r="E273" s="10"/>
+      <c r="H273" s="10"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
       <c r="A274" s="10"/>
       <c r="E274" s="10"/>
+      <c r="H274" s="10"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
       <c r="A275" s="10"/>
       <c r="E275" s="10"/>
+      <c r="H275" s="10"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
       <c r="A276" s="10"/>
       <c r="E276" s="10"/>
+      <c r="H276" s="10"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
       <c r="A277" s="10"/>
       <c r="E277" s="10"/>
+      <c r="H277" s="10"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
       <c r="A278" s="10"/>
       <c r="E278" s="10"/>
+      <c r="H278" s="10"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
       <c r="A279" s="10"/>
       <c r="E279" s="10"/>
+      <c r="H279" s="10"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
       <c r="A280" s="10"/>
       <c r="E280" s="10"/>
+      <c r="H280" s="10"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
       <c r="A281" s="10"/>
       <c r="E281" s="10"/>
+      <c r="H281" s="10"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
       <c r="A282" s="10"/>
       <c r="E282" s="10"/>
+      <c r="H282" s="10"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
       <c r="A283" s="10"/>
       <c r="E283" s="10"/>
+      <c r="H283" s="10"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
       <c r="A284" s="10"/>
       <c r="E284" s="10"/>
+      <c r="H284" s="10"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
       <c r="A285" s="10"/>
       <c r="E285" s="10"/>
+      <c r="H285" s="10"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
       <c r="A286" s="10"/>
       <c r="E286" s="10"/>
+      <c r="H286" s="10"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
       <c r="A287" s="10"/>
       <c r="E287" s="10"/>
+      <c r="H287" s="10"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
       <c r="A288" s="10"/>
       <c r="E288" s="10"/>
+      <c r="H288" s="10"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
       <c r="A289" s="10"/>
       <c r="E289" s="10"/>
+      <c r="H289" s="10"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
       <c r="A290" s="10"/>
       <c r="E290" s="10"/>
+      <c r="H290" s="10"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
       <c r="A291" s="10"/>
       <c r="E291" s="10"/>
+      <c r="H291" s="10"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
       <c r="A292" s="10"/>
       <c r="E292" s="10"/>
+      <c r="H292" s="10"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
       <c r="A293" s="10"/>
       <c r="E293" s="10"/>
+      <c r="H293" s="10"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
       <c r="A294" s="10"/>
       <c r="E294" s="10"/>
+      <c r="H294" s="10"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
       <c r="A295" s="10"/>
       <c r="E295" s="10"/>
+      <c r="H295" s="10"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
       <c r="A296" s="10"/>
       <c r="E296" s="10"/>
+      <c r="H296" s="10"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
       <c r="A297" s="10"/>
       <c r="E297" s="10"/>
+      <c r="H297" s="10"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
       <c r="A298" s="10"/>
       <c r="E298" s="10"/>
+      <c r="H298" s="10"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
       <c r="A299" s="10"/>
       <c r="E299" s="10"/>
+      <c r="H299" s="10"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
       <c r="A300" s="10"/>
       <c r="E300" s="10"/>
+      <c r="H300" s="10"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
       <c r="A301" s="10"/>
       <c r="E301" s="10"/>
+      <c r="H301" s="10"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
       <c r="A302" s="10"/>
       <c r="E302" s="10"/>
+      <c r="H302" s="10"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
       <c r="A303" s="10"/>
       <c r="E303" s="10"/>
+      <c r="H303" s="10"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
       <c r="A304" s="10"/>
       <c r="E304" s="10"/>
+      <c r="H304" s="10"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
       <c r="A305" s="10"/>
       <c r="E305" s="10"/>
+      <c r="H305" s="10"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
       <c r="A306" s="10"/>
       <c r="E306" s="10"/>
+      <c r="H306" s="10"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
       <c r="A307" s="10"/>
       <c r="E307" s="10"/>
+      <c r="H307" s="10"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
       <c r="A308" s="10"/>
       <c r="E308" s="10"/>
+      <c r="H308" s="10"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
       <c r="A309" s="10"/>
       <c r="E309" s="10"/>
+      <c r="H309" s="10"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
       <c r="A310" s="10"/>
       <c r="E310" s="10"/>
+      <c r="H310" s="10"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
       <c r="A311" s="10"/>
       <c r="E311" s="10"/>
+      <c r="H311" s="10"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
       <c r="A312" s="10"/>
       <c r="E312" s="10"/>
+      <c r="H312" s="10"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
       <c r="A313" s="10"/>
       <c r="E313" s="10"/>
+      <c r="H313" s="10"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
       <c r="A314" s="10"/>
       <c r="E314" s="10"/>
+      <c r="H314" s="10"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="10"/>
       <c r="E315" s="10"/>
+      <c r="H315" s="10"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
       <c r="A316" s="10"/>
       <c r="E316" s="10"/>
+      <c r="H316" s="10"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
       <c r="A317" s="10"/>
       <c r="E317" s="10"/>
+      <c r="H317" s="10"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
       <c r="A318" s="10"/>
       <c r="E318" s="10"/>
+      <c r="H318" s="10"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
       <c r="A319" s="10"/>
       <c r="E319" s="10"/>
+      <c r="H319" s="10"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
       <c r="A320" s="10"/>
       <c r="E320" s="10"/>
+      <c r="H320" s="10"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
       <c r="A321" s="10"/>
       <c r="E321" s="10"/>
+      <c r="H321" s="10"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
       <c r="A322" s="10"/>
       <c r="E322" s="10"/>
+      <c r="H322" s="10"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
       <c r="A323" s="10"/>
       <c r="E323" s="10"/>
+      <c r="H323" s="10"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
       <c r="A324" s="10"/>
       <c r="E324" s="10"/>
+      <c r="H324" s="10"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
       <c r="A325" s="10"/>
       <c r="E325" s="10"/>
+      <c r="H325" s="10"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
       <c r="A326" s="10"/>
       <c r="E326" s="10"/>
+      <c r="H326" s="10"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
       <c r="A327" s="10"/>
       <c r="E327" s="10"/>
+      <c r="H327" s="10"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
       <c r="A328" s="10"/>
       <c r="E328" s="10"/>
+      <c r="H328" s="10"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
       <c r="A329" s="10"/>
       <c r="E329" s="10"/>
+      <c r="H329" s="10"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
       <c r="A330" s="10"/>
       <c r="E330" s="10"/>
+      <c r="H330" s="10"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
       <c r="A331" s="10"/>
       <c r="E331" s="10"/>
+      <c r="H331" s="10"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
       <c r="A332" s="10"/>
       <c r="E332" s="10"/>
+      <c r="H332" s="10"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
       <c r="A333" s="10"/>
       <c r="E333" s="10"/>
+      <c r="H333" s="10"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
       <c r="A334" s="10"/>
       <c r="E334" s="10"/>
+      <c r="H334" s="10"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
       <c r="A335" s="10"/>
       <c r="E335" s="10"/>
+      <c r="H335" s="10"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
       <c r="A336" s="10"/>
       <c r="E336" s="10"/>
+      <c r="H336" s="10"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
       <c r="A337" s="10"/>
       <c r="E337" s="10"/>
+      <c r="H337" s="10"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
       <c r="A338" s="10"/>
       <c r="E338" s="10"/>
+      <c r="H338" s="10"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
       <c r="A339" s="10"/>
       <c r="E339" s="10"/>
+      <c r="H339" s="10"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
       <c r="A340" s="10"/>
       <c r="E340" s="10"/>
+      <c r="H340" s="10"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
       <c r="A341" s="10"/>
       <c r="E341" s="10"/>
+      <c r="H341" s="10"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
       <c r="A342" s="10"/>
       <c r="E342" s="10"/>
+      <c r="H342" s="10"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
       <c r="A343" s="10"/>
       <c r="E343" s="10"/>
+      <c r="H343" s="10"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
       <c r="A344" s="10"/>
       <c r="E344" s="10"/>
+      <c r="H344" s="10"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
       <c r="A345" s="10"/>
       <c r="E345" s="10"/>
+      <c r="H345" s="10"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
       <c r="A346" s="10"/>
       <c r="E346" s="10"/>
+      <c r="H346" s="10"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
       <c r="A347" s="10"/>
       <c r="E347" s="10"/>
+      <c r="H347" s="10"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
       <c r="A348" s="10"/>
       <c r="E348" s="10"/>
+      <c r="H348" s="10"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
       <c r="A349" s="10"/>
       <c r="E349" s="10"/>
+      <c r="H349" s="10"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
       <c r="A350" s="10"/>
       <c r="E350" s="10"/>
+      <c r="H350" s="10"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
       <c r="A351" s="10"/>
       <c r="E351" s="10"/>
+      <c r="H351" s="10"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
       <c r="A352" s="10"/>
       <c r="E352" s="10"/>
+      <c r="H352" s="10"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
       <c r="A353" s="10"/>
       <c r="E353" s="10"/>
+      <c r="H353" s="10"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
       <c r="A354" s="10"/>
       <c r="E354" s="10"/>
+      <c r="H354" s="10"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
       <c r="A355" s="10"/>
       <c r="E355" s="10"/>
+      <c r="H355" s="10"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
       <c r="A356" s="10"/>
       <c r="E356" s="10"/>
+      <c r="H356" s="10"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
       <c r="A357" s="10"/>
       <c r="E357" s="10"/>
+      <c r="H357" s="10"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
       <c r="A358" s="10"/>
       <c r="E358" s="10"/>
+      <c r="H358" s="10"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
       <c r="A359" s="10"/>
       <c r="E359" s="10"/>
+      <c r="H359" s="10"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
       <c r="A360" s="10"/>
       <c r="E360" s="10"/>
+      <c r="H360" s="10"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
       <c r="A361" s="10"/>
       <c r="E361" s="10"/>
+      <c r="H361" s="10"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
       <c r="A362" s="10"/>
       <c r="E362" s="10"/>
+      <c r="H362" s="10"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
       <c r="A363" s="10"/>
       <c r="E363" s="10"/>
+      <c r="H363" s="10"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
       <c r="A364" s="10"/>
       <c r="E364" s="10"/>
+      <c r="H364" s="10"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
       <c r="A365" s="10"/>
       <c r="E365" s="10"/>
+      <c r="H365" s="10"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
       <c r="A366" s="10"/>
       <c r="E366" s="10"/>
+      <c r="H366" s="10"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
       <c r="A367" s="10"/>
       <c r="E367" s="10"/>
+      <c r="H367" s="10"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
       <c r="A368" s="10"/>
       <c r="E368" s="10"/>
+      <c r="H368" s="10"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
       <c r="A369" s="10"/>
       <c r="E369" s="10"/>
+      <c r="H369" s="10"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
       <c r="A370" s="10"/>
       <c r="E370" s="10"/>
+      <c r="H370" s="10"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
       <c r="A371" s="10"/>
       <c r="E371" s="10"/>
+      <c r="H371" s="10"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
       <c r="A372" s="10"/>
       <c r="E372" s="10"/>
+      <c r="H372" s="10"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
       <c r="A373" s="10"/>
       <c r="E373" s="10"/>
+      <c r="H373" s="10"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
       <c r="A374" s="10"/>
       <c r="E374" s="10"/>
+      <c r="H374" s="10"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
       <c r="A375" s="10"/>
       <c r="E375" s="10"/>
+      <c r="H375" s="10"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
       <c r="A376" s="10"/>
       <c r="E376" s="10"/>
+      <c r="H376" s="10"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
       <c r="A377" s="10"/>
       <c r="E377" s="10"/>
+      <c r="H377" s="10"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
       <c r="A378" s="10"/>
       <c r="E378" s="10"/>
+      <c r="H378" s="10"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
       <c r="A379" s="10"/>
       <c r="E379" s="10"/>
+      <c r="H379" s="10"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
       <c r="A380" s="10"/>
       <c r="E380" s="10"/>
+      <c r="H380" s="10"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
       <c r="A381" s="10"/>
       <c r="E381" s="10"/>
+      <c r="H381" s="10"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
       <c r="A382" s="10"/>
       <c r="E382" s="10"/>
+      <c r="H382" s="10"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
       <c r="A383" s="10"/>
       <c r="E383" s="10"/>
+      <c r="H383" s="10"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
       <c r="A384" s="10"/>
       <c r="E384" s="10"/>
+      <c r="H384" s="10"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
       <c r="A385" s="10"/>
       <c r="E385" s="10"/>
+      <c r="H385" s="10"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
       <c r="A386" s="10"/>
       <c r="E386" s="10"/>
+      <c r="H386" s="10"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
       <c r="A387" s="10"/>
       <c r="E387" s="10"/>
+      <c r="H387" s="10"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
       <c r="A388" s="10"/>
       <c r="E388" s="10"/>
+      <c r="H388" s="10"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
       <c r="A389" s="10"/>
       <c r="E389" s="10"/>
+      <c r="H389" s="10"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
       <c r="A390" s="10"/>
       <c r="E390" s="10"/>
+      <c r="H390" s="10"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
       <c r="A391" s="10"/>
       <c r="E391" s="10"/>
+      <c r="H391" s="10"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
       <c r="A392" s="10"/>
       <c r="E392" s="10"/>
+      <c r="H392" s="10"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
       <c r="A393" s="10"/>
       <c r="E393" s="10"/>
+      <c r="H393" s="10"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
       <c r="A394" s="10"/>
       <c r="E394" s="10"/>
+      <c r="H394" s="10"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
       <c r="A395" s="10"/>
       <c r="E395" s="10"/>
+      <c r="H395" s="10"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
       <c r="A396" s="10"/>
       <c r="E396" s="10"/>
+      <c r="H396" s="10"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
       <c r="A397" s="10"/>
       <c r="E397" s="10"/>
+      <c r="H397" s="10"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
       <c r="A398" s="10"/>
       <c r="E398" s="10"/>
+      <c r="H398" s="10"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
       <c r="A399" s="10"/>
       <c r="E399" s="10"/>
+      <c r="H399" s="10"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
       <c r="A400" s="10"/>
       <c r="E400" s="10"/>
+      <c r="H400" s="10"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
       <c r="A401" s="10"/>
       <c r="E401" s="10"/>
+      <c r="H401" s="10"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
       <c r="A402" s="10"/>
       <c r="E402" s="10"/>
+      <c r="H402" s="10"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
       <c r="A403" s="10"/>
       <c r="E403" s="10"/>
+      <c r="H403" s="10"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
       <c r="A404" s="10"/>
       <c r="E404" s="10"/>
+      <c r="H404" s="10"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
       <c r="A405" s="10"/>
       <c r="E405" s="10"/>
+      <c r="H405" s="10"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
       <c r="A406" s="10"/>
       <c r="E406" s="10"/>
+      <c r="H406" s="10"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
       <c r="A407" s="10"/>
       <c r="E407" s="10"/>
+      <c r="H407" s="10"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
       <c r="A408" s="10"/>
       <c r="E408" s="10"/>
+      <c r="H408" s="10"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
       <c r="A409" s="10"/>
       <c r="E409" s="10"/>
+      <c r="H409" s="10"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
       <c r="A410" s="10"/>
       <c r="E410" s="10"/>
+      <c r="H410" s="10"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
       <c r="A411" s="10"/>
       <c r="E411" s="10"/>
+      <c r="H411" s="10"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
       <c r="A412" s="10"/>
       <c r="E412" s="10"/>
+      <c r="H412" s="10"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
       <c r="A413" s="10"/>
       <c r="E413" s="10"/>
+      <c r="H413" s="10"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
       <c r="A414" s="10"/>
       <c r="E414" s="10"/>
+      <c r="H414" s="10"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
       <c r="A415" s="10"/>
       <c r="E415" s="10"/>
+      <c r="H415" s="10"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
       <c r="A416" s="10"/>
       <c r="E416" s="10"/>
+      <c r="H416" s="10"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
       <c r="A417" s="10"/>
       <c r="E417" s="10"/>
+      <c r="H417" s="10"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
       <c r="A418" s="10"/>
       <c r="E418" s="10"/>
+      <c r="H418" s="10"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
       <c r="A419" s="10"/>
       <c r="E419" s="10"/>
+      <c r="H419" s="10"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
       <c r="A420" s="10"/>
       <c r="E420" s="10"/>
+      <c r="H420" s="10"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
       <c r="A421" s="10"/>
       <c r="E421" s="10"/>
+      <c r="H421" s="10"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
       <c r="A422" s="10"/>
       <c r="E422" s="10"/>
+      <c r="H422" s="10"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
       <c r="A423" s="10"/>
       <c r="E423" s="10"/>
+      <c r="H423" s="10"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
       <c r="A424" s="10"/>
       <c r="E424" s="10"/>
+      <c r="H424" s="10"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
       <c r="A425" s="10"/>
       <c r="E425" s="10"/>
+      <c r="H425" s="10"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
       <c r="A426" s="10"/>
       <c r="E426" s="10"/>
+      <c r="H426" s="10"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
       <c r="A427" s="10"/>
       <c r="E427" s="10"/>
+      <c r="H427" s="10"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
       <c r="A428" s="10"/>
       <c r="E428" s="10"/>
+      <c r="H428" s="10"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
       <c r="A429" s="10"/>
       <c r="E429" s="10"/>
+      <c r="H429" s="10"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
       <c r="A430" s="10"/>
       <c r="E430" s="10"/>
+      <c r="H430" s="10"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
       <c r="A431" s="10"/>
       <c r="E431" s="10"/>
+      <c r="H431" s="10"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
       <c r="A432" s="10"/>
       <c r="E432" s="10"/>
+      <c r="H432" s="10"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
       <c r="A433" s="10"/>
       <c r="E433" s="10"/>
+      <c r="H433" s="10"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
       <c r="A434" s="10"/>
       <c r="E434" s="10"/>
+      <c r="H434" s="10"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
       <c r="A435" s="10"/>
       <c r="E435" s="10"/>
+      <c r="H435" s="10"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
       <c r="A436" s="10"/>
       <c r="E436" s="10"/>
+      <c r="H436" s="10"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
       <c r="A437" s="10"/>
       <c r="E437" s="10"/>
+      <c r="H437" s="10"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
       <c r="A438" s="10"/>
       <c r="E438" s="10"/>
+      <c r="H438" s="10"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
       <c r="A439" s="10"/>
       <c r="E439" s="10"/>
+      <c r="H439" s="10"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
       <c r="A440" s="10"/>
       <c r="E440" s="10"/>
+      <c r="H440" s="10"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
       <c r="A441" s="10"/>
       <c r="E441" s="10"/>
+      <c r="H441" s="10"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
       <c r="A442" s="10"/>
       <c r="E442" s="10"/>
+      <c r="H442" s="10"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
       <c r="A443" s="10"/>
       <c r="E443" s="10"/>
+      <c r="H443" s="10"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
       <c r="A444" s="10"/>
       <c r="E444" s="10"/>
+      <c r="H444" s="10"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
       <c r="A445" s="10"/>
       <c r="E445" s="10"/>
+      <c r="H445" s="10"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
       <c r="A446" s="10"/>
       <c r="E446" s="10"/>
+      <c r="H446" s="10"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
       <c r="A447" s="10"/>
       <c r="E447" s="10"/>
+      <c r="H447" s="10"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
       <c r="A448" s="10"/>
       <c r="E448" s="10"/>
+      <c r="H448" s="10"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
       <c r="A449" s="10"/>
       <c r="E449" s="10"/>
+      <c r="H449" s="10"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
       <c r="A450" s="10"/>
       <c r="E450" s="10"/>
+      <c r="H450" s="10"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
       <c r="A451" s="10"/>
       <c r="E451" s="10"/>
+      <c r="H451" s="10"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
       <c r="A452" s="10"/>
       <c r="E452" s="10"/>
+      <c r="H452" s="10"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
       <c r="A453" s="10"/>
       <c r="E453" s="10"/>
+      <c r="H453" s="10"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
       <c r="A454" s="10"/>
       <c r="E454" s="10"/>
+      <c r="H454" s="10"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
       <c r="A455" s="10"/>
       <c r="E455" s="10"/>
+      <c r="H455" s="10"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
       <c r="A456" s="10"/>
       <c r="E456" s="10"/>
+      <c r="H456" s="10"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
       <c r="A457" s="10"/>
       <c r="E457" s="10"/>
+      <c r="H457" s="10"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
       <c r="A458" s="10"/>
       <c r="E458" s="10"/>
+      <c r="H458" s="10"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
       <c r="A459" s="10"/>
       <c r="E459" s="10"/>
+      <c r="H459" s="10"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
       <c r="A460" s="10"/>
       <c r="E460" s="10"/>
+      <c r="H460" s="10"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
       <c r="A461" s="10"/>
       <c r="E461" s="10"/>
+      <c r="H461" s="10"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
       <c r="A462" s="10"/>
       <c r="E462" s="10"/>
+      <c r="H462" s="10"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
       <c r="A463" s="10"/>
       <c r="E463" s="10"/>
+      <c r="H463" s="10"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
       <c r="A464" s="10"/>
       <c r="E464" s="10"/>
+      <c r="H464" s="10"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
       <c r="A465" s="10"/>
       <c r="E465" s="10"/>
+      <c r="H465" s="10"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
       <c r="A466" s="10"/>
       <c r="E466" s="10"/>
+      <c r="H466" s="10"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
       <c r="A467" s="10"/>
       <c r="E467" s="10"/>
+      <c r="H467" s="10"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
       <c r="A468" s="10"/>
       <c r="E468" s="10"/>
+      <c r="H468" s="10"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
       <c r="A469" s="10"/>
       <c r="E469" s="10"/>
+      <c r="H469" s="10"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
       <c r="A470" s="10"/>
       <c r="E470" s="10"/>
+      <c r="H470" s="10"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
       <c r="A471" s="10"/>
       <c r="E471" s="10"/>
+      <c r="H471" s="10"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
       <c r="A472" s="10"/>
       <c r="E472" s="10"/>
+      <c r="H472" s="10"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
       <c r="A473" s="10"/>
       <c r="E473" s="10"/>
+      <c r="H473" s="10"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
       <c r="A474" s="10"/>
       <c r="E474" s="10"/>
+      <c r="H474" s="10"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
       <c r="A475" s="10"/>
       <c r="E475" s="10"/>
+      <c r="H475" s="10"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
       <c r="A476" s="10"/>
       <c r="E476" s="10"/>
+      <c r="H476" s="10"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
       <c r="A477" s="10"/>
       <c r="E477" s="10"/>
+      <c r="H477" s="10"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
       <c r="A478" s="10"/>
       <c r="E478" s="10"/>
+      <c r="H478" s="10"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
       <c r="A479" s="10"/>
       <c r="E479" s="10"/>
+      <c r="H479" s="10"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
       <c r="A480" s="10"/>
       <c r="E480" s="10"/>
+      <c r="H480" s="10"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
       <c r="A481" s="10"/>
       <c r="E481" s="10"/>
+      <c r="H481" s="10"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
       <c r="A482" s="10"/>
       <c r="E482" s="10"/>
+      <c r="H482" s="10"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
       <c r="A483" s="10"/>
       <c r="E483" s="10"/>
+      <c r="H483" s="10"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
       <c r="A484" s="10"/>
       <c r="E484" s="10"/>
+      <c r="H484" s="10"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
       <c r="A485" s="10"/>
       <c r="E485" s="10"/>
+      <c r="H485" s="10"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
       <c r="A486" s="10"/>
       <c r="E486" s="10"/>
+      <c r="H486" s="10"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
       <c r="A487" s="10"/>
       <c r="E487" s="10"/>
+      <c r="H487" s="10"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
       <c r="A488" s="10"/>
       <c r="E488" s="10"/>
+      <c r="H488" s="10"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
       <c r="A489" s="10"/>
       <c r="E489" s="10"/>
+      <c r="H489" s="10"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
       <c r="A490" s="10"/>
       <c r="E490" s="10"/>
+      <c r="H490" s="10"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
       <c r="A491" s="10"/>
       <c r="E491" s="10"/>
+      <c r="H491" s="10"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
       <c r="A492" s="10"/>
       <c r="E492" s="10"/>
+      <c r="H492" s="10"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
       <c r="A493" s="10"/>
       <c r="E493" s="10"/>
+      <c r="H493" s="10"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
       <c r="A494" s="10"/>
       <c r="E494" s="10"/>
+      <c r="H494" s="10"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
       <c r="A495" s="10"/>
       <c r="E495" s="10"/>
+      <c r="H495" s="10"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
       <c r="A496" s="10"/>
       <c r="E496" s="10"/>
+      <c r="H496" s="10"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
       <c r="A497" s="10"/>
       <c r="E497" s="10"/>
+      <c r="H497" s="10"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
       <c r="A498" s="10"/>
       <c r="E498" s="10"/>
+      <c r="H498" s="10"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
       <c r="A499" s="10"/>
       <c r="E499" s="10"/>
+      <c r="H499" s="10"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
       <c r="A500" s="10"/>
       <c r="E500" s="10"/>
+      <c r="H500" s="10"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
       <c r="A501" s="10"/>
       <c r="E501" s="10"/>
+      <c r="H501" s="10"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
       <c r="A502" s="10"/>
       <c r="E502" s="10"/>
+      <c r="H502" s="10"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
       <c r="A503" s="10"/>
       <c r="E503" s="10"/>
+      <c r="H503" s="10"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
       <c r="A504" s="10"/>
       <c r="E504" s="10"/>
+      <c r="H504" s="10"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
       <c r="A505" s="10"/>
       <c r="E505" s="10"/>
+      <c r="H505" s="10"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
       <c r="A506" s="10"/>
       <c r="E506" s="10"/>
+      <c r="H506" s="10"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
       <c r="A507" s="10"/>
       <c r="E507" s="10"/>
+      <c r="H507" s="10"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
       <c r="A508" s="10"/>
       <c r="E508" s="10"/>
+      <c r="H508" s="10"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
       <c r="A509" s="10"/>
       <c r="E509" s="10"/>
+      <c r="H509" s="10"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
       <c r="A510" s="10"/>
       <c r="E510" s="10"/>
+      <c r="H510" s="10"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
       <c r="A511" s="10"/>
       <c r="E511" s="10"/>
+      <c r="H511" s="10"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
       <c r="A512" s="10"/>
       <c r="E512" s="10"/>
+      <c r="H512" s="10"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
       <c r="A513" s="10"/>
       <c r="E513" s="10"/>
+      <c r="H513" s="10"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
       <c r="A514" s="10"/>
       <c r="E514" s="10"/>
+      <c r="H514" s="10"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
       <c r="A515" s="10"/>
       <c r="E515" s="10"/>
+      <c r="H515" s="10"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
       <c r="A516" s="10"/>
       <c r="E516" s="10"/>
+      <c r="H516" s="10"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
       <c r="A517" s="10"/>
       <c r="E517" s="10"/>
+      <c r="H517" s="10"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
       <c r="A518" s="10"/>
       <c r="E518" s="10"/>
+      <c r="H518" s="10"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
       <c r="A519" s="10"/>
       <c r="E519" s="10"/>
+      <c r="H519" s="10"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
       <c r="A520" s="10"/>
       <c r="E520" s="10"/>
+      <c r="H520" s="10"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
       <c r="A521" s="10"/>
       <c r="E521" s="10"/>
+      <c r="H521" s="10"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
       <c r="A522" s="10"/>
       <c r="E522" s="10"/>
+      <c r="H522" s="10"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
       <c r="A523" s="10"/>
       <c r="E523" s="10"/>
+      <c r="H523" s="10"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
       <c r="A524" s="10"/>
       <c r="E524" s="10"/>
+      <c r="H524" s="10"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
       <c r="A525" s="10"/>
       <c r="E525" s="10"/>
+      <c r="H525" s="10"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
       <c r="A526" s="10"/>
       <c r="E526" s="10"/>
+      <c r="H526" s="10"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
       <c r="A527" s="10"/>
       <c r="E527" s="10"/>
+      <c r="H527" s="10"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
       <c r="A528" s="10"/>
       <c r="E528" s="10"/>
+      <c r="H528" s="10"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
       <c r="A529" s="10"/>
       <c r="E529" s="10"/>
+      <c r="H529" s="10"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
       <c r="A530" s="10"/>
       <c r="E530" s="10"/>
+      <c r="H530" s="10"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
       <c r="A531" s="10"/>
       <c r="E531" s="10"/>
+      <c r="H531" s="10"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
       <c r="A532" s="10"/>
       <c r="E532" s="10"/>
+      <c r="H532" s="10"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
       <c r="A533" s="10"/>
       <c r="E533" s="10"/>
+      <c r="H533" s="10"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
       <c r="A534" s="10"/>
       <c r="E534" s="10"/>
+      <c r="H534" s="10"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
       <c r="A535" s="10"/>
       <c r="E535" s="10"/>
+      <c r="H535" s="10"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
       <c r="A536" s="10"/>
       <c r="E536" s="10"/>
+      <c r="H536" s="10"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
       <c r="A537" s="10"/>
       <c r="E537" s="10"/>
+      <c r="H537" s="10"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
       <c r="A538" s="10"/>
       <c r="E538" s="10"/>
+      <c r="H538" s="10"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
       <c r="A539" s="10"/>
       <c r="E539" s="10"/>
+      <c r="H539" s="10"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
       <c r="A540" s="10"/>
       <c r="E540" s="10"/>
+      <c r="H540" s="10"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
       <c r="A541" s="10"/>
       <c r="E541" s="10"/>
+      <c r="H541" s="10"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
       <c r="A542" s="10"/>
       <c r="E542" s="10"/>
+      <c r="H542" s="10"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
       <c r="A543" s="10"/>
       <c r="E543" s="10"/>
+      <c r="H543" s="10"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
       <c r="A544" s="10"/>
       <c r="E544" s="10"/>
+      <c r="H544" s="10"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
       <c r="A545" s="10"/>
       <c r="E545" s="10"/>
+      <c r="H545" s="10"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
       <c r="A546" s="10"/>
       <c r="E546" s="10"/>
+      <c r="H546" s="10"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
       <c r="A547" s="10"/>
       <c r="E547" s="10"/>
+      <c r="H547" s="10"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
       <c r="A548" s="10"/>
       <c r="E548" s="10"/>
+      <c r="H548" s="10"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
       <c r="A549" s="10"/>
       <c r="E549" s="10"/>
+      <c r="H549" s="10"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
       <c r="A550" s="10"/>
       <c r="E550" s="10"/>
+      <c r="H550" s="10"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
       <c r="A551" s="10"/>
       <c r="E551" s="10"/>
+      <c r="H551" s="10"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
       <c r="A552" s="10"/>
       <c r="E552" s="10"/>
+      <c r="H552" s="10"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
       <c r="A553" s="10"/>
       <c r="E553" s="10"/>
+      <c r="H553" s="10"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
       <c r="A554" s="10"/>
       <c r="E554" s="10"/>
+      <c r="H554" s="10"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
       <c r="A555" s="10"/>
       <c r="E555" s="10"/>
+      <c r="H555" s="10"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
       <c r="A556" s="10"/>
       <c r="E556" s="10"/>
+      <c r="H556" s="10"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
       <c r="A557" s="10"/>
       <c r="E557" s="10"/>
+      <c r="H557" s="10"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
       <c r="A558" s="10"/>
       <c r="E558" s="10"/>
+      <c r="H558" s="10"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
       <c r="A559" s="10"/>
       <c r="E559" s="10"/>
+      <c r="H559" s="10"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
       <c r="A560" s="10"/>
       <c r="E560" s="10"/>
+      <c r="H560" s="10"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
       <c r="A561" s="10"/>
       <c r="E561" s="10"/>
+      <c r="H561" s="10"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
       <c r="A562" s="10"/>
       <c r="E562" s="10"/>
+      <c r="H562" s="10"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
       <c r="A563" s="10"/>
       <c r="E563" s="10"/>
+      <c r="H563" s="10"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
       <c r="A564" s="10"/>
       <c r="E564" s="10"/>
+      <c r="H564" s="10"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
       <c r="A565" s="10"/>
       <c r="E565" s="10"/>
+      <c r="H565" s="10"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
       <c r="A566" s="10"/>
       <c r="E566" s="10"/>
+      <c r="H566" s="10"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
       <c r="A567" s="10"/>
       <c r="E567" s="10"/>
+      <c r="H567" s="10"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
       <c r="A568" s="10"/>
       <c r="E568" s="10"/>
+      <c r="H568" s="10"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
       <c r="A569" s="10"/>
       <c r="E569" s="10"/>
+      <c r="H569" s="10"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
       <c r="A570" s="10"/>
       <c r="E570" s="10"/>
+      <c r="H570" s="10"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
       <c r="A571" s="10"/>
       <c r="E571" s="10"/>
+      <c r="H571" s="10"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
       <c r="A572" s="10"/>
       <c r="E572" s="10"/>
+      <c r="H572" s="10"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
       <c r="A573" s="10"/>
       <c r="E573" s="10"/>
+      <c r="H573" s="10"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
       <c r="A574" s="10"/>
       <c r="E574" s="10"/>
+      <c r="H574" s="10"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
       <c r="A575" s="10"/>
       <c r="E575" s="10"/>
+      <c r="H575" s="10"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
       <c r="A576" s="10"/>
       <c r="E576" s="10"/>
+      <c r="H576" s="10"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
       <c r="A577" s="10"/>
       <c r="E577" s="10"/>
+      <c r="H577" s="10"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
       <c r="A578" s="10"/>
       <c r="E578" s="10"/>
+      <c r="H578" s="10"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
       <c r="A579" s="10"/>
       <c r="E579" s="10"/>
+      <c r="H579" s="10"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
       <c r="A580" s="10"/>
       <c r="E580" s="10"/>
+      <c r="H580" s="10"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
       <c r="A581" s="10"/>
       <c r="E581" s="10"/>
+      <c r="H581" s="10"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
       <c r="A582" s="10"/>
       <c r="E582" s="10"/>
+      <c r="H582" s="10"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
       <c r="A583" s="10"/>
       <c r="E583" s="10"/>
+      <c r="H583" s="10"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
       <c r="A584" s="10"/>
       <c r="E584" s="10"/>
+      <c r="H584" s="10"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
       <c r="A585" s="10"/>
       <c r="E585" s="10"/>
+      <c r="H585" s="10"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
       <c r="A586" s="10"/>
       <c r="E586" s="10"/>
+      <c r="H586" s="10"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
       <c r="A587" s="10"/>
       <c r="E587" s="10"/>
+      <c r="H587" s="10"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
       <c r="A588" s="10"/>
       <c r="E588" s="10"/>
+      <c r="H588" s="10"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
       <c r="A589" s="10"/>
       <c r="E589" s="10"/>
+      <c r="H589" s="10"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
       <c r="A590" s="10"/>
       <c r="E590" s="10"/>
+      <c r="H590" s="10"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
       <c r="A591" s="10"/>
       <c r="E591" s="10"/>
+      <c r="H591" s="10"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
       <c r="A592" s="10"/>
       <c r="E592" s="10"/>
+      <c r="H592" s="10"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
       <c r="A593" s="10"/>
       <c r="E593" s="10"/>
+      <c r="H593" s="10"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
       <c r="A594" s="10"/>
       <c r="E594" s="10"/>
+      <c r="H594" s="10"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
       <c r="A595" s="10"/>
       <c r="E595" s="10"/>
+      <c r="H595" s="10"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
       <c r="A596" s="10"/>
       <c r="E596" s="10"/>
+      <c r="H596" s="10"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
       <c r="A597" s="10"/>
       <c r="E597" s="10"/>
+      <c r="H597" s="10"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
       <c r="A598" s="10"/>
       <c r="E598" s="10"/>
+      <c r="H598" s="10"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
       <c r="A599" s="10"/>
       <c r="E599" s="10"/>
+      <c r="H599" s="10"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
       <c r="A600" s="10"/>
       <c r="E600" s="10"/>
+      <c r="H600" s="10"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
       <c r="A601" s="10"/>
       <c r="E601" s="10"/>
+      <c r="H601" s="10"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
       <c r="A602" s="10"/>
       <c r="E602" s="10"/>
+      <c r="H602" s="10"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
       <c r="A603" s="10"/>
       <c r="E603" s="10"/>
+      <c r="H603" s="10"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
       <c r="A604" s="10"/>
       <c r="E604" s="10"/>
+      <c r="H604" s="10"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
       <c r="A605" s="10"/>
       <c r="E605" s="10"/>
+      <c r="H605" s="10"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
       <c r="A606" s="10"/>
       <c r="E606" s="10"/>
+      <c r="H606" s="10"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
       <c r="A607" s="10"/>
       <c r="E607" s="10"/>
+      <c r="H607" s="10"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
       <c r="A608" s="10"/>
       <c r="E608" s="10"/>
+      <c r="H608" s="10"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
       <c r="A609" s="10"/>
       <c r="E609" s="10"/>
+      <c r="H609" s="10"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
       <c r="A610" s="10"/>
       <c r="E610" s="10"/>
+      <c r="H610" s="10"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
       <c r="A611" s="10"/>
       <c r="E611" s="10"/>
+      <c r="H611" s="10"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
       <c r="A612" s="10"/>
       <c r="E612" s="10"/>
+      <c r="H612" s="10"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
       <c r="A613" s="10"/>
       <c r="E613" s="10"/>
+      <c r="H613" s="10"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
       <c r="A614" s="10"/>
       <c r="E614" s="10"/>
+      <c r="H614" s="10"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
       <c r="A615" s="10"/>
       <c r="E615" s="10"/>
+      <c r="H615" s="10"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
       <c r="A616" s="10"/>
       <c r="E616" s="10"/>
+      <c r="H616" s="10"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
       <c r="A617" s="10"/>
       <c r="E617" s="10"/>
+      <c r="H617" s="10"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
       <c r="A618" s="10"/>
       <c r="E618" s="10"/>
+      <c r="H618" s="10"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
       <c r="A619" s="10"/>
       <c r="E619" s="10"/>
+      <c r="H619" s="10"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
       <c r="A620" s="10"/>
       <c r="E620" s="10"/>
+      <c r="H620" s="10"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
       <c r="A621" s="10"/>
       <c r="E621" s="10"/>
+      <c r="H621" s="10"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
       <c r="A622" s="10"/>
       <c r="E622" s="10"/>
+      <c r="H622" s="10"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
       <c r="A623" s="10"/>
       <c r="E623" s="10"/>
+      <c r="H623" s="10"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
       <c r="A624" s="10"/>
       <c r="E624" s="10"/>
+      <c r="H624" s="10"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
       <c r="A625" s="10"/>
       <c r="E625" s="10"/>
+      <c r="H625" s="10"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
       <c r="A626" s="10"/>
       <c r="E626" s="10"/>
+      <c r="H626" s="10"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
       <c r="A627" s="10"/>
       <c r="E627" s="10"/>
+      <c r="H627" s="10"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
       <c r="A628" s="10"/>
       <c r="E628" s="10"/>
+      <c r="H628" s="10"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
       <c r="A629" s="10"/>
       <c r="E629" s="10"/>
+      <c r="H629" s="10"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
       <c r="A630" s="10"/>
       <c r="E630" s="10"/>
+      <c r="H630" s="10"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
       <c r="A631" s="10"/>
       <c r="E631" s="10"/>
+      <c r="H631" s="10"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
       <c r="A632" s="10"/>
       <c r="E632" s="10"/>
+      <c r="H632" s="10"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
       <c r="A633" s="10"/>
       <c r="E633" s="10"/>
+      <c r="H633" s="10"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
       <c r="A634" s="10"/>
       <c r="E634" s="10"/>
+      <c r="H634" s="10"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
       <c r="A635" s="10"/>
       <c r="E635" s="10"/>
+      <c r="H635" s="10"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
       <c r="A636" s="10"/>
       <c r="E636" s="10"/>
+      <c r="H636" s="10"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
       <c r="A637" s="10"/>
       <c r="E637" s="10"/>
+      <c r="H637" s="10"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
       <c r="A638" s="10"/>
       <c r="E638" s="10"/>
+      <c r="H638" s="10"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
       <c r="A639" s="10"/>
       <c r="E639" s="10"/>
+      <c r="H639" s="10"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
       <c r="A640" s="10"/>
       <c r="E640" s="10"/>
+      <c r="H640" s="10"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
       <c r="A641" s="10"/>
       <c r="E641" s="10"/>
+      <c r="H641" s="10"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
       <c r="A642" s="10"/>
       <c r="E642" s="10"/>
+      <c r="H642" s="10"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
       <c r="A643" s="10"/>
       <c r="E643" s="10"/>
+      <c r="H643" s="10"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
       <c r="A644" s="10"/>
       <c r="E644" s="10"/>
+      <c r="H644" s="10"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
       <c r="A645" s="10"/>
       <c r="E645" s="10"/>
+      <c r="H645" s="10"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
       <c r="A646" s="10"/>
       <c r="E646" s="10"/>
+      <c r="H646" s="10"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
       <c r="A647" s="10"/>
       <c r="E647" s="10"/>
+      <c r="H647" s="10"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
       <c r="A648" s="10"/>
       <c r="E648" s="10"/>
+      <c r="H648" s="10"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
       <c r="A649" s="10"/>
       <c r="E649" s="10"/>
+      <c r="H649" s="10"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
       <c r="A650" s="10"/>
       <c r="E650" s="10"/>
+      <c r="H650" s="10"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
       <c r="A651" s="10"/>
       <c r="E651" s="10"/>
+      <c r="H651" s="10"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
       <c r="A652" s="10"/>
       <c r="E652" s="10"/>
+      <c r="H652" s="10"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
       <c r="A653" s="10"/>
       <c r="E653" s="10"/>
+      <c r="H653" s="10"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
       <c r="A654" s="10"/>
       <c r="E654" s="10"/>
+      <c r="H654" s="10"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
       <c r="A655" s="10"/>
       <c r="E655" s="10"/>
+      <c r="H655" s="10"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
       <c r="A656" s="10"/>
       <c r="E656" s="10"/>
+      <c r="H656" s="10"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
       <c r="A657" s="10"/>
       <c r="E657" s="10"/>
+      <c r="H657" s="10"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
       <c r="A658" s="10"/>
       <c r="E658" s="10"/>
+      <c r="H658" s="10"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
       <c r="A659" s="10"/>
       <c r="E659" s="10"/>
+      <c r="H659" s="10"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
       <c r="A660" s="10"/>
       <c r="E660" s="10"/>
+      <c r="H660" s="10"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
       <c r="A661" s="10"/>
       <c r="E661" s="10"/>
+      <c r="H661" s="10"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
       <c r="A662" s="10"/>
       <c r="E662" s="10"/>
+      <c r="H662" s="10"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
       <c r="A663" s="10"/>
       <c r="E663" s="10"/>
+      <c r="H663" s="10"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
       <c r="A664" s="10"/>
       <c r="E664" s="10"/>
+      <c r="H664" s="10"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
       <c r="A665" s="10"/>
       <c r="E665" s="10"/>
+      <c r="H665" s="10"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
       <c r="A666" s="10"/>
       <c r="E666" s="10"/>
+      <c r="H666" s="10"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
       <c r="A667" s="10"/>
       <c r="E667" s="10"/>
+      <c r="H667" s="10"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
       <c r="A668" s="10"/>
       <c r="E668" s="10"/>
+      <c r="H668" s="10"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
       <c r="A669" s="10"/>
       <c r="E669" s="10"/>
+      <c r="H669" s="10"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
       <c r="A670" s="10"/>
       <c r="E670" s="10"/>
+      <c r="H670" s="10"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
       <c r="A671" s="10"/>
       <c r="E671" s="10"/>
+      <c r="H671" s="10"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
       <c r="A672" s="10"/>
       <c r="E672" s="10"/>
+      <c r="H672" s="10"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
       <c r="A673" s="10"/>
       <c r="E673" s="10"/>
+      <c r="H673" s="10"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
       <c r="A674" s="10"/>
       <c r="E674" s="10"/>
+      <c r="H674" s="10"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
       <c r="A675" s="10"/>
       <c r="E675" s="10"/>
+      <c r="H675" s="10"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
       <c r="A676" s="10"/>
       <c r="E676" s="10"/>
+      <c r="H676" s="10"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
       <c r="A677" s="10"/>
       <c r="E677" s="10"/>
+      <c r="H677" s="10"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
       <c r="A678" s="10"/>
       <c r="E678" s="10"/>
+      <c r="H678" s="10"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
       <c r="A679" s="10"/>
       <c r="E679" s="10"/>
+      <c r="H679" s="10"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
       <c r="A680" s="10"/>
       <c r="E680" s="10"/>
+      <c r="H680" s="10"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
       <c r="A681" s="10"/>
       <c r="E681" s="10"/>
+      <c r="H681" s="10"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
       <c r="A682" s="10"/>
       <c r="E682" s="10"/>
+      <c r="H682" s="10"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
       <c r="A683" s="10"/>
       <c r="E683" s="10"/>
+      <c r="H683" s="10"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
       <c r="A684" s="10"/>
       <c r="E684" s="10"/>
+      <c r="H684" s="10"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
       <c r="A685" s="10"/>
       <c r="E685" s="10"/>
+      <c r="H685" s="10"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
       <c r="A686" s="10"/>
       <c r="E686" s="10"/>
+      <c r="H686" s="10"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
       <c r="A687" s="10"/>
       <c r="E687" s="10"/>
+      <c r="H687" s="10"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
       <c r="A688" s="10"/>
       <c r="E688" s="10"/>
+      <c r="H688" s="10"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
       <c r="A689" s="10"/>
       <c r="E689" s="10"/>
+      <c r="H689" s="10"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
       <c r="A690" s="10"/>
       <c r="E690" s="10"/>
+      <c r="H690" s="10"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
       <c r="A691" s="10"/>
       <c r="E691" s="10"/>
+      <c r="H691" s="10"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
       <c r="A692" s="10"/>
       <c r="E692" s="10"/>
+      <c r="H692" s="10"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
       <c r="A693" s="10"/>
       <c r="E693" s="10"/>
+      <c r="H693" s="10"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
       <c r="A694" s="10"/>
       <c r="E694" s="10"/>
+      <c r="H694" s="10"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
       <c r="A695" s="10"/>
       <c r="E695" s="10"/>
+      <c r="H695" s="10"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
       <c r="A696" s="10"/>
       <c r="E696" s="10"/>
+      <c r="H696" s="10"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
       <c r="A697" s="10"/>
       <c r="E697" s="10"/>
+      <c r="H697" s="10"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
       <c r="A698" s="10"/>
       <c r="E698" s="10"/>
+      <c r="H698" s="10"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
       <c r="A699" s="10"/>
       <c r="E699" s="10"/>
+      <c r="H699" s="10"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
       <c r="A700" s="10"/>
       <c r="E700" s="10"/>
+      <c r="H700" s="10"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
       <c r="A701" s="10"/>
       <c r="E701" s="10"/>
+      <c r="H701" s="10"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
       <c r="A702" s="10"/>
       <c r="E702" s="10"/>
+      <c r="H702" s="10"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
       <c r="A703" s="10"/>
       <c r="E703" s="10"/>
+      <c r="H703" s="10"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
       <c r="A704" s="10"/>
       <c r="E704" s="10"/>
+      <c r="H704" s="10"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
       <c r="A705" s="10"/>
       <c r="E705" s="10"/>
+      <c r="H705" s="10"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
       <c r="A706" s="10"/>
       <c r="E706" s="10"/>
+      <c r="H706" s="10"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
       <c r="A707" s="10"/>
       <c r="E707" s="10"/>
+      <c r="H707" s="10"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
       <c r="A708" s="10"/>
       <c r="E708" s="10"/>
+      <c r="H708" s="10"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
       <c r="A709" s="10"/>
       <c r="E709" s="10"/>
+      <c r="H709" s="10"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
       <c r="A710" s="10"/>
       <c r="E710" s="10"/>
+      <c r="H710" s="10"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
       <c r="A711" s="10"/>
       <c r="E711" s="10"/>
+      <c r="H711" s="10"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
       <c r="A712" s="10"/>
       <c r="E712" s="10"/>
+      <c r="H712" s="10"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
       <c r="A713" s="10"/>
       <c r="E713" s="10"/>
+      <c r="H713" s="10"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
       <c r="A714" s="10"/>
       <c r="E714" s="10"/>
+      <c r="H714" s="10"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
       <c r="A715" s="10"/>
       <c r="E715" s="10"/>
+      <c r="H715" s="10"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
       <c r="A716" s="10"/>
       <c r="E716" s="10"/>
+      <c r="H716" s="10"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
       <c r="A717" s="10"/>
       <c r="E717" s="10"/>
+      <c r="H717" s="10"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
       <c r="A718" s="10"/>
       <c r="E718" s="10"/>
+      <c r="H718" s="10"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
       <c r="A719" s="10"/>
       <c r="E719" s="10"/>
+      <c r="H719" s="10"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
       <c r="A720" s="10"/>
       <c r="E720" s="10"/>
+      <c r="H720" s="10"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
       <c r="A721" s="10"/>
       <c r="E721" s="10"/>
+      <c r="H721" s="10"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
       <c r="A722" s="10"/>
       <c r="E722" s="10"/>
+      <c r="H722" s="10"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
       <c r="A723" s="10"/>
       <c r="E723" s="10"/>
+      <c r="H723" s="10"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
       <c r="A724" s="10"/>
       <c r="E724" s="10"/>
+      <c r="H724" s="10"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
       <c r="A725" s="10"/>
       <c r="E725" s="10"/>
+      <c r="H725" s="10"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
       <c r="A726" s="10"/>
       <c r="E726" s="10"/>
+      <c r="H726" s="10"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
       <c r="A727" s="10"/>
       <c r="E727" s="10"/>
+      <c r="H727" s="10"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
       <c r="A728" s="10"/>
       <c r="E728" s="10"/>
+      <c r="H728" s="10"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
       <c r="A729" s="10"/>
       <c r="E729" s="10"/>
+      <c r="H729" s="10"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
       <c r="A730" s="10"/>
       <c r="E730" s="10"/>
+      <c r="H730" s="10"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
       <c r="A731" s="10"/>
       <c r="E731" s="10"/>
+      <c r="H731" s="10"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
       <c r="A732" s="10"/>
       <c r="E732" s="10"/>
+      <c r="H732" s="10"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
       <c r="A733" s="10"/>
       <c r="E733" s="10"/>
+      <c r="H733" s="10"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
       <c r="A734" s="10"/>
       <c r="E734" s="10"/>
+      <c r="H734" s="10"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
       <c r="A735" s="10"/>
       <c r="E735" s="10"/>
+      <c r="H735" s="10"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
       <c r="A736" s="10"/>
       <c r="E736" s="10"/>
+      <c r="H736" s="10"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
       <c r="A737" s="10"/>
       <c r="E737" s="10"/>
+      <c r="H737" s="10"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
       <c r="A738" s="10"/>
       <c r="E738" s="10"/>
+      <c r="H738" s="10"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
       <c r="A739" s="10"/>
       <c r="E739" s="10"/>
+      <c r="H739" s="10"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
       <c r="A740" s="10"/>
       <c r="E740" s="10"/>
+      <c r="H740" s="10"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
       <c r="A741" s="10"/>
       <c r="E741" s="10"/>
+      <c r="H741" s="10"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
       <c r="A742" s="10"/>
       <c r="E742" s="10"/>
+      <c r="H742" s="10"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
       <c r="A743" s="10"/>
       <c r="E743" s="10"/>
+      <c r="H743" s="10"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
       <c r="A744" s="10"/>
       <c r="E744" s="10"/>
+      <c r="H744" s="10"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
       <c r="A745" s="10"/>
       <c r="E745" s="10"/>
+      <c r="H745" s="10"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
       <c r="A746" s="10"/>
       <c r="E746" s="10"/>
+      <c r="H746" s="10"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
       <c r="A747" s="10"/>
       <c r="E747" s="10"/>
+      <c r="H747" s="10"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
       <c r="A748" s="10"/>
       <c r="E748" s="10"/>
+      <c r="H748" s="10"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
       <c r="A749" s="10"/>
       <c r="E749" s="10"/>
+      <c r="H749" s="10"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
       <c r="A750" s="10"/>
       <c r="E750" s="10"/>
+      <c r="H750" s="10"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
       <c r="A751" s="10"/>
       <c r="E751" s="10"/>
+      <c r="H751" s="10"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
       <c r="A752" s="10"/>
       <c r="E752" s="10"/>
+      <c r="H752" s="10"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
       <c r="A753" s="10"/>
       <c r="E753" s="10"/>
+      <c r="H753" s="10"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
       <c r="A754" s="10"/>
       <c r="E754" s="10"/>
+      <c r="H754" s="10"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
       <c r="A755" s="10"/>
       <c r="E755" s="10"/>
+      <c r="H755" s="10"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
       <c r="A756" s="10"/>
       <c r="E756" s="10"/>
+      <c r="H756" s="10"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
       <c r="A757" s="10"/>
       <c r="E757" s="10"/>
+      <c r="H757" s="10"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
       <c r="A758" s="10"/>
       <c r="E758" s="10"/>
+      <c r="H758" s="10"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
       <c r="A759" s="10"/>
       <c r="E759" s="10"/>
+      <c r="H759" s="10"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
       <c r="A760" s="10"/>
       <c r="E760" s="10"/>
+      <c r="H760" s="10"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
       <c r="A761" s="10"/>
       <c r="E761" s="10"/>
+      <c r="H761" s="10"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
       <c r="A762" s="10"/>
       <c r="E762" s="10"/>
+      <c r="H762" s="10"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
       <c r="A763" s="10"/>
       <c r="E763" s="10"/>
+      <c r="H763" s="10"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
       <c r="A764" s="10"/>
       <c r="E764" s="10"/>
+      <c r="H764" s="10"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
       <c r="A765" s="10"/>
       <c r="E765" s="10"/>
+      <c r="H765" s="10"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
       <c r="A766" s="10"/>
       <c r="E766" s="10"/>
+      <c r="H766" s="10"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
       <c r="A767" s="10"/>
       <c r="E767" s="10"/>
+      <c r="H767" s="10"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
       <c r="A768" s="10"/>
       <c r="E768" s="10"/>
+      <c r="H768" s="10"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
       <c r="A769" s="10"/>
       <c r="E769" s="10"/>
+      <c r="H769" s="10"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
       <c r="A770" s="10"/>
       <c r="E770" s="10"/>
+      <c r="H770" s="10"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
       <c r="A771" s="10"/>
       <c r="E771" s="10"/>
+      <c r="H771" s="10"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
       <c r="A772" s="10"/>
       <c r="E772" s="10"/>
+      <c r="H772" s="10"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
       <c r="A773" s="10"/>
       <c r="E773" s="10"/>
+      <c r="H773" s="10"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
       <c r="A774" s="10"/>
       <c r="E774" s="10"/>
+      <c r="H774" s="10"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
       <c r="A775" s="10"/>
       <c r="E775" s="10"/>
+      <c r="H775" s="10"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
       <c r="A776" s="10"/>
       <c r="E776" s="10"/>
+      <c r="H776" s="10"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
       <c r="A777" s="10"/>
       <c r="E777" s="10"/>
+      <c r="H777" s="10"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
       <c r="A778" s="10"/>
       <c r="E778" s="10"/>
+      <c r="H778" s="10"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
       <c r="A779" s="10"/>
       <c r="E779" s="10"/>
+      <c r="H779" s="10"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
       <c r="A780" s="10"/>
       <c r="E780" s="10"/>
+      <c r="H780" s="10"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
       <c r="A781" s="10"/>
       <c r="E781" s="10"/>
+      <c r="H781" s="10"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
       <c r="A782" s="10"/>
       <c r="E782" s="10"/>
+      <c r="H782" s="10"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
       <c r="A783" s="10"/>
       <c r="E783" s="10"/>
+      <c r="H783" s="10"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
       <c r="A784" s="10"/>
       <c r="E784" s="10"/>
+      <c r="H784" s="10"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
       <c r="A785" s="10"/>
       <c r="E785" s="10"/>
+      <c r="H785" s="10"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
       <c r="A786" s="10"/>
       <c r="E786" s="10"/>
+      <c r="H786" s="10"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
       <c r="A787" s="10"/>
       <c r="E787" s="10"/>
+      <c r="H787" s="10"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
       <c r="A788" s="10"/>
       <c r="E788" s="10"/>
+      <c r="H788" s="10"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
       <c r="A789" s="10"/>
       <c r="E789" s="10"/>
+      <c r="H789" s="10"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
       <c r="A790" s="10"/>
       <c r="E790" s="10"/>
+      <c r="H790" s="10"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
       <c r="A791" s="10"/>
       <c r="E791" s="10"/>
+      <c r="H791" s="10"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
       <c r="A792" s="10"/>
       <c r="E792" s="10"/>
+      <c r="H792" s="10"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
       <c r="A793" s="10"/>
       <c r="E793" s="10"/>
+      <c r="H793" s="10"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
       <c r="A794" s="10"/>
       <c r="E794" s="10"/>
+      <c r="H794" s="10"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
       <c r="A795" s="10"/>
       <c r="E795" s="10"/>
+      <c r="H795" s="10"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
       <c r="A796" s="10"/>
       <c r="E796" s="10"/>
+      <c r="H796" s="10"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
       <c r="A797" s="10"/>
       <c r="E797" s="10"/>
+      <c r="H797" s="10"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
       <c r="A798" s="10"/>
       <c r="E798" s="10"/>
+      <c r="H798" s="10"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
       <c r="A799" s="10"/>
       <c r="E799" s="10"/>
+      <c r="H799" s="10"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
       <c r="A800" s="10"/>
       <c r="E800" s="10"/>
+      <c r="H800" s="10"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
       <c r="A801" s="10"/>
       <c r="E801" s="10"/>
+      <c r="H801" s="10"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
       <c r="A802" s="10"/>
       <c r="E802" s="10"/>
+      <c r="H802" s="10"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
       <c r="A803" s="10"/>
       <c r="E803" s="10"/>
+      <c r="H803" s="10"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
       <c r="A804" s="10"/>
       <c r="E804" s="10"/>
+      <c r="H804" s="10"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
       <c r="A805" s="10"/>
       <c r="E805" s="10"/>
+      <c r="H805" s="10"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
       <c r="A806" s="10"/>
       <c r="E806" s="10"/>
+      <c r="H806" s="10"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
       <c r="A807" s="10"/>
       <c r="E807" s="10"/>
+      <c r="H807" s="10"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
       <c r="A808" s="10"/>
       <c r="E808" s="10"/>
+      <c r="H808" s="10"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
       <c r="A809" s="10"/>
       <c r="E809" s="10"/>
+      <c r="H809" s="10"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
       <c r="A810" s="10"/>
       <c r="E810" s="10"/>
+      <c r="H810" s="10"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
       <c r="A811" s="10"/>
       <c r="E811" s="10"/>
+      <c r="H811" s="10"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
       <c r="A812" s="10"/>
       <c r="E812" s="10"/>
+      <c r="H812" s="10"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
       <c r="A813" s="10"/>
       <c r="E813" s="10"/>
+      <c r="H813" s="10"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
       <c r="A814" s="10"/>
       <c r="E814" s="10"/>
+      <c r="H814" s="10"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
       <c r="A815" s="10"/>
       <c r="E815" s="10"/>
+      <c r="H815" s="10"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
       <c r="A816" s="10"/>
       <c r="E816" s="10"/>
+      <c r="H816" s="10"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
       <c r="A817" s="10"/>
       <c r="E817" s="10"/>
+      <c r="H817" s="10"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
       <c r="A818" s="10"/>
       <c r="E818" s="10"/>
+      <c r="H818" s="10"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
       <c r="A819" s="10"/>
       <c r="E819" s="10"/>
+      <c r="H819" s="10"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
       <c r="A820" s="10"/>
       <c r="E820" s="10"/>
+      <c r="H820" s="10"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
       <c r="A821" s="10"/>
       <c r="E821" s="10"/>
+      <c r="H821" s="10"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
       <c r="A822" s="10"/>
       <c r="E822" s="10"/>
+      <c r="H822" s="10"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
       <c r="A823" s="10"/>
       <c r="E823" s="10"/>
+      <c r="H823" s="10"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
       <c r="A824" s="10"/>
       <c r="E824" s="10"/>
+      <c r="H824" s="10"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
       <c r="A825" s="10"/>
       <c r="E825" s="10"/>
+      <c r="H825" s="10"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
       <c r="A826" s="10"/>
       <c r="E826" s="10"/>
+      <c r="H826" s="10"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
       <c r="A827" s="10"/>
       <c r="E827" s="10"/>
+      <c r="H827" s="10"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
       <c r="A828" s="10"/>
       <c r="E828" s="10"/>
+      <c r="H828" s="10"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
       <c r="A829" s="10"/>
       <c r="E829" s="10"/>
+      <c r="H829" s="10"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
       <c r="A830" s="10"/>
       <c r="E830" s="10"/>
+      <c r="H830" s="10"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
       <c r="A831" s="10"/>
       <c r="E831" s="10"/>
+      <c r="H831" s="10"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
       <c r="A832" s="10"/>
       <c r="E832" s="10"/>
+      <c r="H832" s="10"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
       <c r="A833" s="10"/>
       <c r="E833" s="10"/>
+      <c r="H833" s="10"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
       <c r="A834" s="10"/>
       <c r="E834" s="10"/>
+      <c r="H834" s="10"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
       <c r="A835" s="10"/>
       <c r="E835" s="10"/>
+      <c r="H835" s="10"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
       <c r="A836" s="10"/>
       <c r="E836" s="10"/>
+      <c r="H836" s="10"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
       <c r="A837" s="10"/>
       <c r="E837" s="10"/>
+      <c r="H837" s="10"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
       <c r="A838" s="10"/>
       <c r="E838" s="10"/>
+      <c r="H838" s="10"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
       <c r="A839" s="10"/>
       <c r="E839" s="10"/>
+      <c r="H839" s="10"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
       <c r="A840" s="10"/>
       <c r="E840" s="10"/>
+      <c r="H840" s="10"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
       <c r="A841" s="10"/>
       <c r="E841" s="10"/>
+      <c r="H841" s="10"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
       <c r="A842" s="10"/>
       <c r="E842" s="10"/>
+      <c r="H842" s="10"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
       <c r="A843" s="10"/>
       <c r="E843" s="10"/>
+      <c r="H843" s="10"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
       <c r="A844" s="10"/>
       <c r="E844" s="10"/>
+      <c r="H844" s="10"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
       <c r="A845" s="10"/>
       <c r="E845" s="10"/>
+      <c r="H845" s="10"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
       <c r="A846" s="10"/>
       <c r="E846" s="10"/>
+      <c r="H846" s="10"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
       <c r="A847" s="10"/>
       <c r="E847" s="10"/>
+      <c r="H847" s="10"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
       <c r="A848" s="10"/>
       <c r="E848" s="10"/>
+      <c r="H848" s="10"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
       <c r="A849" s="10"/>
       <c r="E849" s="10"/>
+      <c r="H849" s="10"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
       <c r="A850" s="10"/>
       <c r="E850" s="10"/>
+      <c r="H850" s="10"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
       <c r="A851" s="10"/>
       <c r="E851" s="10"/>
+      <c r="H851" s="10"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
       <c r="A852" s="10"/>
       <c r="E852" s="10"/>
+      <c r="H852" s="10"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
       <c r="A853" s="10"/>
       <c r="E853" s="10"/>
+      <c r="H853" s="10"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
       <c r="A854" s="10"/>
       <c r="E854" s="10"/>
+      <c r="H854" s="10"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
       <c r="A855" s="10"/>
       <c r="E855" s="10"/>
+      <c r="H855" s="10"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
       <c r="A856" s="10"/>
       <c r="E856" s="10"/>
+      <c r="H856" s="10"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
       <c r="A857" s="10"/>
       <c r="E857" s="10"/>
+      <c r="H857" s="10"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
       <c r="A858" s="10"/>
       <c r="E858" s="10"/>
+      <c r="H858" s="10"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
       <c r="A859" s="10"/>
       <c r="E859" s="10"/>
+      <c r="H859" s="10"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
       <c r="A860" s="10"/>
       <c r="E860" s="10"/>
+      <c r="H860" s="10"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
       <c r="A861" s="10"/>
       <c r="E861" s="10"/>
+      <c r="H861" s="10"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
       <c r="A862" s="10"/>
       <c r="E862" s="10"/>
+      <c r="H862" s="10"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
       <c r="A863" s="10"/>
       <c r="E863" s="10"/>
+      <c r="H863" s="10"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
       <c r="A864" s="10"/>
       <c r="E864" s="10"/>
+      <c r="H864" s="10"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
       <c r="A865" s="10"/>
       <c r="E865" s="10"/>
+      <c r="H865" s="10"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
       <c r="A866" s="10"/>
       <c r="E866" s="10"/>
+      <c r="H866" s="10"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
       <c r="A867" s="10"/>
       <c r="E867" s="10"/>
+      <c r="H867" s="10"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
       <c r="A868" s="10"/>
       <c r="E868" s="10"/>
+      <c r="H868" s="10"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
       <c r="A869" s="10"/>
       <c r="E869" s="10"/>
+      <c r="H869" s="10"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
       <c r="A870" s="10"/>
       <c r="E870" s="10"/>
+      <c r="H870" s="10"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
       <c r="A871" s="10"/>
       <c r="E871" s="10"/>
+      <c r="H871" s="10"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
       <c r="A872" s="10"/>
       <c r="E872" s="10"/>
+      <c r="H872" s="10"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
       <c r="A873" s="10"/>
       <c r="E873" s="10"/>
+      <c r="H873" s="10"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
       <c r="A874" s="10"/>
       <c r="E874" s="10"/>
+      <c r="H874" s="10"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
       <c r="A875" s="10"/>
       <c r="E875" s="10"/>
+      <c r="H875" s="10"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
       <c r="A876" s="10"/>
       <c r="E876" s="10"/>
+      <c r="H876" s="10"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
       <c r="A877" s="10"/>
       <c r="E877" s="10"/>
+      <c r="H877" s="10"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
       <c r="A878" s="10"/>
       <c r="E878" s="10"/>
+      <c r="H878" s="10"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
       <c r="A879" s="10"/>
       <c r="E879" s="10"/>
+      <c r="H879" s="10"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
       <c r="A880" s="10"/>
       <c r="E880" s="10"/>
+      <c r="H880" s="10"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
       <c r="A881" s="10"/>
       <c r="E881" s="10"/>
+      <c r="H881" s="10"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
       <c r="A882" s="10"/>
       <c r="E882" s="10"/>
+      <c r="H882" s="10"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
       <c r="A883" s="10"/>
       <c r="E883" s="10"/>
+      <c r="H883" s="10"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
       <c r="A884" s="10"/>
       <c r="E884" s="10"/>
+      <c r="H884" s="10"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
       <c r="A885" s="10"/>
       <c r="E885" s="10"/>
+      <c r="H885" s="10"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
       <c r="A886" s="10"/>
       <c r="E886" s="10"/>
+      <c r="H886" s="10"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
       <c r="A887" s="10"/>
       <c r="E887" s="10"/>
+      <c r="H887" s="10"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
       <c r="A888" s="10"/>
       <c r="E888" s="10"/>
+      <c r="H888" s="10"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
       <c r="A889" s="10"/>
       <c r="E889" s="10"/>
+      <c r="H889" s="10"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
       <c r="A890" s="10"/>
       <c r="E890" s="10"/>
+      <c r="H890" s="10"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
       <c r="A891" s="10"/>
       <c r="E891" s="10"/>
+      <c r="H891" s="10"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
       <c r="A892" s="10"/>
       <c r="E892" s="10"/>
+      <c r="H892" s="10"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
       <c r="A893" s="10"/>
       <c r="E893" s="10"/>
+      <c r="H893" s="10"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
       <c r="A894" s="10"/>
       <c r="E894" s="10"/>
+      <c r="H894" s="10"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
       <c r="A895" s="10"/>
       <c r="E895" s="10"/>
+      <c r="H895" s="10"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
       <c r="A896" s="10"/>
       <c r="E896" s="10"/>
+      <c r="H896" s="10"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
       <c r="A897" s="10"/>
       <c r="E897" s="10"/>
+      <c r="H897" s="10"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
       <c r="A898" s="10"/>
       <c r="E898" s="10"/>
+      <c r="H898" s="10"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
       <c r="A899" s="10"/>
       <c r="E899" s="10"/>
+      <c r="H899" s="10"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
       <c r="A900" s="10"/>
       <c r="E900" s="10"/>
+      <c r="H900" s="10"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
       <c r="A901" s="10"/>
       <c r="E901" s="10"/>
+      <c r="H901" s="10"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
       <c r="A902" s="10"/>
       <c r="E902" s="10"/>
+      <c r="H902" s="10"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
       <c r="A903" s="10"/>
       <c r="E903" s="10"/>
+      <c r="H903" s="10"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
       <c r="A904" s="10"/>
       <c r="E904" s="10"/>
+      <c r="H904" s="10"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
       <c r="A905" s="10"/>
       <c r="E905" s="10"/>
+      <c r="H905" s="10"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
       <c r="A906" s="10"/>
       <c r="E906" s="10"/>
+      <c r="H906" s="10"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
       <c r="A907" s="10"/>
       <c r="E907" s="10"/>
+      <c r="H907" s="10"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
       <c r="A908" s="10"/>
       <c r="E908" s="10"/>
+      <c r="H908" s="10"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
       <c r="A909" s="10"/>
       <c r="E909" s="10"/>
+      <c r="H909" s="10"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
       <c r="A910" s="10"/>
       <c r="E910" s="10"/>
+      <c r="H910" s="10"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
       <c r="A911" s="10"/>
       <c r="E911" s="10"/>
+      <c r="H911" s="10"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
       <c r="A912" s="10"/>
       <c r="E912" s="10"/>
+      <c r="H912" s="10"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
       <c r="A913" s="10"/>
       <c r="E913" s="10"/>
+      <c r="H913" s="10"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
       <c r="A914" s="10"/>
       <c r="E914" s="10"/>
+      <c r="H914" s="10"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
       <c r="A915" s="10"/>
       <c r="E915" s="10"/>
+      <c r="H915" s="10"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
       <c r="A916" s="10"/>
       <c r="E916" s="10"/>
+      <c r="H916" s="10"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
       <c r="A917" s="10"/>
       <c r="E917" s="10"/>
+      <c r="H917" s="10"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
       <c r="A918" s="10"/>
       <c r="E918" s="10"/>
+      <c r="H918" s="10"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
       <c r="A919" s="10"/>
       <c r="E919" s="10"/>
+      <c r="H919" s="10"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
       <c r="A920" s="10"/>
       <c r="E920" s="10"/>
+      <c r="H920" s="10"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
       <c r="A921" s="10"/>
       <c r="E921" s="10"/>
+      <c r="H921" s="10"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
       <c r="A922" s="10"/>
       <c r="E922" s="10"/>
+      <c r="H922" s="10"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
       <c r="A923" s="10"/>
       <c r="E923" s="10"/>
+      <c r="H923" s="10"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
       <c r="A924" s="10"/>
       <c r="E924" s="10"/>
+      <c r="H924" s="10"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
       <c r="A925" s="10"/>
       <c r="E925" s="10"/>
+      <c r="H925" s="10"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
       <c r="A926" s="10"/>
       <c r="E926" s="10"/>
+      <c r="H926" s="10"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
       <c r="A927" s="10"/>
       <c r="E927" s="10"/>
+      <c r="H927" s="10"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
       <c r="A928" s="10"/>
       <c r="E928" s="10"/>
+      <c r="H928" s="10"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
       <c r="A929" s="10"/>
       <c r="E929" s="10"/>
+      <c r="H929" s="10"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
       <c r="A930" s="10"/>
       <c r="E930" s="10"/>
+      <c r="H930" s="10"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
       <c r="A931" s="10"/>
       <c r="E931" s="10"/>
+      <c r="H931" s="10"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
       <c r="A932" s="10"/>
       <c r="E932" s="10"/>
+      <c r="H932" s="10"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
       <c r="A933" s="10"/>
       <c r="E933" s="10"/>
+      <c r="H933" s="10"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
       <c r="A934" s="10"/>
       <c r="E934" s="10"/>
+      <c r="H934" s="10"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
       <c r="A935" s="10"/>
       <c r="E935" s="10"/>
+      <c r="H935" s="10"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
       <c r="A936" s="10"/>
       <c r="E936" s="10"/>
+      <c r="H936" s="10"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
       <c r="A937" s="10"/>
       <c r="E937" s="10"/>
+      <c r="H937" s="10"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
       <c r="A938" s="10"/>
       <c r="E938" s="10"/>
+      <c r="H938" s="10"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
       <c r="A939" s="10"/>
       <c r="E939" s="10"/>
+      <c r="H939" s="10"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
       <c r="A940" s="10"/>
       <c r="E940" s="10"/>
+      <c r="H940" s="10"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
       <c r="A941" s="10"/>
       <c r="E941" s="10"/>
+      <c r="H941" s="10"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
       <c r="A942" s="10"/>
       <c r="E942" s="10"/>
+      <c r="H942" s="10"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
       <c r="A943" s="10"/>
       <c r="E943" s="10"/>
+      <c r="H943" s="10"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
       <c r="A944" s="10"/>
       <c r="E944" s="10"/>
+      <c r="H944" s="10"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
       <c r="A945" s="10"/>
       <c r="E945" s="10"/>
+      <c r="H945" s="10"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
       <c r="A946" s="10"/>
       <c r="E946" s="10"/>
+      <c r="H946" s="10"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
       <c r="A947" s="10"/>
       <c r="E947" s="10"/>
+      <c r="H947" s="10"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
       <c r="A948" s="10"/>
       <c r="E948" s="10"/>
+      <c r="H948" s="10"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
       <c r="A949" s="10"/>
       <c r="E949" s="10"/>
+      <c r="H949" s="10"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
       <c r="A950" s="10"/>
       <c r="E950" s="10"/>
+      <c r="H950" s="10"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
       <c r="A951" s="10"/>
       <c r="E951" s="10"/>
+      <c r="H951" s="10"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
       <c r="A952" s="10"/>
       <c r="E952" s="10"/>
+      <c r="H952" s="10"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
       <c r="A953" s="10"/>
       <c r="E953" s="10"/>
+      <c r="H953" s="10"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
       <c r="A954" s="10"/>
       <c r="E954" s="10"/>
+      <c r="H954" s="10"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
       <c r="A955" s="10"/>
       <c r="E955" s="10"/>
+      <c r="H955" s="10"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
       <c r="A956" s="10"/>
       <c r="E956" s="10"/>
+      <c r="H956" s="10"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
       <c r="A957" s="10"/>
       <c r="E957" s="10"/>
+      <c r="H957" s="10"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
       <c r="A958" s="10"/>
       <c r="E958" s="10"/>
+      <c r="H958" s="10"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
       <c r="A959" s="10"/>
       <c r="E959" s="10"/>
+      <c r="H959" s="10"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
       <c r="A960" s="10"/>
       <c r="E960" s="10"/>
+      <c r="H960" s="10"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
       <c r="A961" s="10"/>
       <c r="E961" s="10"/>
+      <c r="H961" s="10"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
       <c r="A962" s="10"/>
       <c r="E962" s="10"/>
+      <c r="H962" s="10"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
       <c r="A963" s="10"/>
       <c r="E963" s="10"/>
+      <c r="H963" s="10"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
       <c r="A964" s="10"/>
       <c r="E964" s="10"/>
+      <c r="H964" s="10"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
       <c r="A965" s="10"/>
       <c r="E965" s="10"/>
+      <c r="H965" s="10"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
       <c r="A966" s="10"/>
       <c r="E966" s="10"/>
+      <c r="H966" s="10"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
       <c r="A967" s="10"/>
       <c r="E967" s="10"/>
+      <c r="H967" s="10"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
       <c r="A968" s="10"/>
       <c r="E968" s="10"/>
+      <c r="H968" s="10"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
       <c r="A969" s="10"/>
       <c r="E969" s="10"/>
+      <c r="H969" s="10"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
       <c r="A970" s="10"/>
       <c r="E970" s="10"/>
+      <c r="H970" s="10"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
       <c r="A971" s="10"/>
       <c r="E971" s="10"/>
+      <c r="H971" s="10"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
       <c r="A972" s="10"/>
       <c r="E972" s="10"/>
+      <c r="H972" s="10"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
       <c r="A973" s="10"/>
       <c r="E973" s="10"/>
+      <c r="H973" s="10"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
       <c r="A974" s="10"/>
       <c r="E974" s="10"/>
+      <c r="H974" s="10"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
       <c r="A975" s="10"/>
       <c r="E975" s="10"/>
+      <c r="H975" s="10"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
       <c r="A976" s="10"/>
       <c r="E976" s="10"/>
+      <c r="H976" s="10"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
       <c r="A977" s="10"/>
       <c r="E977" s="10"/>
+      <c r="H977" s="10"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
       <c r="A978" s="10"/>
       <c r="E978" s="10"/>
+      <c r="H978" s="10"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
       <c r="A979" s="10"/>
       <c r="E979" s="10"/>
+      <c r="H979" s="10"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
       <c r="A980" s="10"/>
       <c r="E980" s="10"/>
+      <c r="H980" s="10"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
       <c r="A981" s="10"/>
       <c r="E981" s="10"/>
+      <c r="H981" s="10"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
       <c r="A982" s="10"/>
       <c r="E982" s="10"/>
+      <c r="H982" s="10"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
       <c r="A983" s="10"/>
       <c r="E983" s="10"/>
+      <c r="H983" s="10"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
       <c r="A984" s="10"/>
       <c r="E984" s="10"/>
+      <c r="H984" s="10"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
       <c r="A985" s="10"/>
       <c r="E985" s="10"/>
+      <c r="H985" s="10"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
       <c r="A986" s="10"/>
       <c r="E986" s="10"/>
+      <c r="H986" s="10"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
       <c r="A987" s="10"/>
       <c r="E987" s="10"/>
+      <c r="H987" s="10"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
       <c r="A988" s="10"/>
       <c r="E988" s="10"/>
+      <c r="H988" s="10"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
       <c r="A989" s="10"/>
       <c r="E989" s="10"/>
+      <c r="H989" s="10"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
       <c r="A990" s="10"/>
       <c r="E990" s="10"/>
+      <c r="H990" s="10"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
       <c r="A991" s="10"/>
       <c r="E991" s="10"/>
+      <c r="H991" s="10"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
       <c r="A992" s="10"/>
       <c r="E992" s="10"/>
+      <c r="H992" s="10"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
       <c r="A993" s="10"/>
       <c r="E993" s="10"/>
+      <c r="H993" s="10"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
       <c r="A994" s="10"/>
       <c r="E994" s="10"/>
+      <c r="H994" s="10"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
       <c r="A995" s="10"/>
       <c r="E995" s="10"/>
+      <c r="H995" s="10"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
       <c r="A996" s="10"/>
       <c r="E996" s="10"/>
+      <c r="H996" s="10"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
       <c r="A997" s="10"/>
       <c r="E997" s="10"/>
+      <c r="H997" s="10"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
       <c r="A998" s="10"/>
       <c r="E998" s="10"/>
+      <c r="H998" s="10"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
       <c r="A999" s="10"/>
       <c r="E999" s="10"/>
+      <c r="H999" s="10"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
       <c r="A1000" s="10"/>
       <c r="E1000" s="10"/>
+      <c r="H1000" s="10"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2">
       <formula1>"0001-For Remelting,0002-Loan from Customer,0015-Qty to Scrap,0018-Service Purpose,0201-Vendor Issue,0202-202 Wrong Entry,0204-Qty to Remelt"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"1200,1300,1150,1210,1250,1000"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H1000">
+      <formula1>"INHOUSE,SUBCONTRACT,DOMESTIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E1000">
+      <formula1>"0001-For Remelting,0015-Qty to Scrap,0017-Scrap Stock Raise,0018-Service Purpose,0016-Return to Vendor,0202-201 Wrong Entry,0203-NPD STOCK RAISE,0204-Qty to Remelt,0205-Dsgn,teststock rais,0206-Salvage frmcust ret,0207-Scrao frm Cust ret,0208-FOC to Custo"&amp;"mer,0209-Loan from Customer"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>

</xml_diff>